<commit_message>
todo: change table to AgGrid
</commit_message>
<xml_diff>
--- a/static/JPMorgan_5-ETF-holdings.xlsx
+++ b/static/JPMorgan_5-ETF-holdings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\ETF-Dashboard\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E1CF208-2E21-40CC-B3CD-DBDD14932EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866DE7D1-8CC1-4692-9190-EEA231627039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" activeTab="4" xr2:uid="{B03D5609-CDFA-4982-8DDA-8AE6E20F0557}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{B03D5609-CDFA-4982-8DDA-8AE6E20F0557}"/>
   </bookViews>
   <sheets>
     <sheet name="JEPI US Equity" sheetId="1" r:id="rId1"/>
@@ -9482,8 +9482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD5C077-166D-433C-A4E9-FBAAE7A5CEEB}">
   <dimension ref="A1:R139"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -69973,11 +69973,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA6C6101-0E06-4D7F-A5AC-19B3DCC0C15A}">
   <dimension ref="A1:R260"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2000" max="2000" width="2.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">

</xml_diff>